<commit_message>
* nightly commit #2
</commit_message>
<xml_diff>
--- a/hardware/power_budget.xlsx
+++ b/hardware/power_budget.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>VCC</t>
   </si>
@@ -189,6 +189,9 @@
   </si>
   <si>
     <t>0.779A (1.35V SSTL 50% TX/RX)</t>
+  </si>
+  <si>
+    <t>V12</t>
   </si>
 </sst>
 </file>
@@ -403,7 +406,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -437,6 +440,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -719,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:AG44"/>
+  <dimension ref="B4:AG45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1122,7 @@
         <v>0.12</v>
       </c>
       <c r="AA9" s="19">
-        <f t="shared" ref="AA9:AA14" si="0">SUM(E9:Y9)</f>
+        <f t="shared" ref="AA9:AA15" si="0">SUM(E9:Y9)</f>
         <v>2.0400000000000009</v>
       </c>
       <c r="AB9" s="18">
@@ -1138,10 +1142,10 @@
     </row>
     <row r="10" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10">
-        <v>0.67500000000000004</v>
+        <v>12</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1153,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1208,1349 +1212,1436 @@
       </c>
       <c r="AA10" s="19">
         <f t="shared" si="0"/>
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="AB10" s="18">
         <f>AA10</f>
-        <v>1.6</v>
-      </c>
-      <c r="AC10" s="17">
-        <v>3</v>
-      </c>
-      <c r="AD10" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="17"/>
+      <c r="AD10" s="26" t="s">
         <v>43</v>
       </c>
       <c r="AE10">
         <f>AC10*2.5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="D11" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1.6</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>0</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="19">
+        <f t="shared" si="0"/>
+        <v>1.6</v>
+      </c>
+      <c r="AB11" s="18">
+        <f>AA11</f>
+        <v>1.6</v>
+      </c>
+      <c r="AC11" s="17">
+        <v>3</v>
+      </c>
+      <c r="AD11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE11">
+        <f>AC11*2.5</f>
         <v>7.5</v>
       </c>
     </row>
-    <row r="11" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="12" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>1.35</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D12" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>0</v>
-      </c>
-      <c r="J11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="K11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="L11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="M11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="N11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="O11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="P11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Q11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="R11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="S11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="T11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="U11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="V11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="W11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="X11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Y11" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="AA11" s="13">
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="K12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="L12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="N12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="O12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="P12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Q12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="R12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="S12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="V12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="W12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="X12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Y12" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AA12" s="13">
         <f t="shared" si="0"/>
         <v>1.3120000000000001</v>
       </c>
     </row>
-    <row r="12" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
+    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>1.35</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D13" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12" s="12">
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
         <v>0.32400000000000001</v>
       </c>
-      <c r="J12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="K12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="L12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="M12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="N12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="O12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="P12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Q12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="R12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="S12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="T12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="U12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="V12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="W12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="X12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Y12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="AA12" s="14">
+      <c r="J13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="K13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="L13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="N13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="O13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="P13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Q13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="R13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="S13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="V13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="W13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="X13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Y13" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AA13" s="14">
         <f t="shared" si="0"/>
         <v>1.6360000000000003</v>
       </c>
     </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
+    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C13">
+      <c r="C14">
         <v>1.35</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D14" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
         <v>1.6</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <f>0.198*16</f>
         <v>3.1680000000000001</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I14" s="12">
         <v>0.32400000000000001</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J14" s="2">
         <v>1.016</v>
       </c>
-      <c r="K13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="L13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="M13" s="2">
+      <c r="K14" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="L14" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M14" s="2">
         <v>1.016</v>
       </c>
-      <c r="N13" s="2">
+      <c r="N14" s="2">
         <v>1.016</v>
       </c>
-      <c r="O13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="P13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Q13" s="2">
+      <c r="O14" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="P14" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Q14" s="2">
         <v>1.016</v>
       </c>
-      <c r="R13" s="2">
+      <c r="R14" s="2">
         <v>1.016</v>
       </c>
-      <c r="S13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="T13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="U13" s="2">
+      <c r="S14" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T14" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U14" s="2">
         <v>1.016</v>
       </c>
-      <c r="V13" s="2">
+      <c r="V14" s="2">
         <v>1.016</v>
       </c>
-      <c r="W13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="X13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Y13" s="2">
+      <c r="W14" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="X14" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Y14" s="2">
         <v>1.016</v>
       </c>
-      <c r="AA13" s="14">
+      <c r="AA14" s="14">
         <f t="shared" si="0"/>
         <v>13.876000000000005</v>
       </c>
-      <c r="AB13" s="4"/>
-      <c r="AC13" s="4"/>
-    </row>
-    <row r="14" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20" t="s">
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4"/>
+    </row>
+    <row r="15" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C14">
+      <c r="C15">
         <v>1.35</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D15" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14" s="12">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12">
         <v>0.32400000000000001</v>
       </c>
-      <c r="J14" s="8">
+      <c r="J15" s="8">
         <v>1.016</v>
       </c>
-      <c r="K14" s="8">
+      <c r="K15" s="8">
         <v>1.016</v>
       </c>
-      <c r="L14" s="8">
+      <c r="L15" s="8">
         <v>1.016</v>
       </c>
-      <c r="M14" s="8">
+      <c r="M15" s="8">
         <v>1.016</v>
       </c>
-      <c r="N14" s="8">
+      <c r="N15" s="8">
         <v>1.016</v>
       </c>
-      <c r="O14" s="8">
+      <c r="O15" s="8">
         <v>1.016</v>
       </c>
-      <c r="P14" s="8">
+      <c r="P15" s="8">
         <v>1.016</v>
       </c>
-      <c r="Q14" s="8">
+      <c r="Q15" s="27">
         <v>1.016</v>
       </c>
-      <c r="R14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="S14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="T14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="U14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="V14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="W14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="X14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Y14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="AA14" s="15">
+      <c r="R15" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="S15" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T15" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U15" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="V15" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="W15" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="X15" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Y15" s="20">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AA15" s="15">
         <f t="shared" si="0"/>
         <v>9.1080000000000059</v>
       </c>
-      <c r="AB14" s="16">
-        <f>SUM(AA11:AA14)</f>
+      <c r="AB15" s="16">
+        <f>SUM(AA12:AA15)</f>
         <v>25.932000000000009</v>
       </c>
-      <c r="AC14" s="17">
+      <c r="AC15" s="17">
         <v>14</v>
       </c>
-      <c r="AD14" s="26" t="s">
+      <c r="AD15" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="AE14">
-        <f>AC14*2*1.35</f>
+      <c r="AE15">
+        <f>AC15*2*1.35</f>
         <v>37.800000000000004</v>
       </c>
-      <c r="AF14">
-        <f>SUM(AE7:AE14)</f>
+      <c r="AF15">
+        <f>SUM(AE7:AE15)</f>
         <v>113.85</v>
       </c>
-      <c r="AG14">
-        <f>AF14/0.9</f>
+      <c r="AG15">
+        <f>AF15/0.9</f>
         <v>126.49999999999999</v>
       </c>
     </row>
-    <row r="15" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="N16" s="25" t="s">
+    <row r="16" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="N17" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="AF16" t="s">
+      <c r="AF17" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="AF17" t="s">
+    <row r="18" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="AF18" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="19" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="E19" s="9" t="s">
+    <row r="20" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="9"/>
-      <c r="V19" s="9"/>
-      <c r="W19" s="9"/>
-      <c r="X19" s="9"/>
-      <c r="Y19" s="9"/>
-    </row>
-    <row r="20" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="E20" s="10" t="str">
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
+      <c r="Y20" s="9"/>
+    </row>
+    <row r="21" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="E21" s="10" t="str">
         <f>E5</f>
         <v>MCU</v>
       </c>
-      <c r="F20" s="10" t="str">
+      <c r="F21" s="10" t="str">
         <f>F5</f>
         <v>Clock Buffer</v>
       </c>
-      <c r="G20" s="10" t="str">
+      <c r="G21" s="10" t="str">
         <f>G5</f>
         <v>Misc</v>
       </c>
-      <c r="H20" s="10" t="str">
-        <f t="shared" ref="H20:Y20" si="1">H5</f>
+      <c r="H21" s="10" t="str">
+        <f t="shared" ref="H21:Y21" si="1">H5</f>
         <v>SDRAM x16</v>
       </c>
-      <c r="I20" s="10" t="str">
+      <c r="I21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-CFG</v>
       </c>
-      <c r="J20" s="10" t="str">
+      <c r="J21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-00</v>
       </c>
-      <c r="K20" s="10" t="str">
+      <c r="K21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-01</v>
       </c>
-      <c r="L20" s="10" t="str">
+      <c r="L21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-02</v>
       </c>
-      <c r="M20" s="10" t="str">
+      <c r="M21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-03</v>
       </c>
-      <c r="N20" s="10" t="str">
+      <c r="N21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-30</v>
       </c>
-      <c r="O20" s="10" t="str">
+      <c r="O21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-31</v>
       </c>
-      <c r="P20" s="10" t="str">
+      <c r="P21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-32</v>
       </c>
-      <c r="Q20" s="10" t="str">
+      <c r="Q21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-33</v>
       </c>
-      <c r="R20" s="10" t="str">
+      <c r="R21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-10</v>
       </c>
-      <c r="S20" s="10" t="str">
+      <c r="S21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-11</v>
       </c>
-      <c r="T20" s="10" t="str">
+      <c r="T21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-12</v>
       </c>
-      <c r="U20" s="10" t="str">
+      <c r="U21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-13</v>
       </c>
-      <c r="V20" s="10" t="str">
+      <c r="V21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-20</v>
       </c>
-      <c r="W20" s="10" t="str">
+      <c r="W21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-21</v>
       </c>
-      <c r="X20" s="10" t="str">
+      <c r="X21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-22</v>
       </c>
-      <c r="Y20" s="10" t="str">
+      <c r="Y21" s="10" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-23</v>
       </c>
     </row>
-    <row r="21" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D21" s="22"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="23"/>
-      <c r="P21" s="23"/>
-      <c r="Q21" s="23"/>
-      <c r="R21" s="23"/>
-      <c r="S21" s="23"/>
-      <c r="T21" s="23"/>
-      <c r="U21" s="23"/>
-      <c r="V21" s="23"/>
-      <c r="W21" s="23"/>
-      <c r="X21" s="23"/>
-      <c r="Y21" s="23"/>
-    </row>
     <row r="22" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="22"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="23"/>
+      <c r="T22" s="23"/>
+      <c r="U22" s="23"/>
+      <c r="V22" s="23"/>
+      <c r="W22" s="23"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+    </row>
+    <row r="23" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D23" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E23" s="4">
         <f>E7*$C7</f>
         <v>1.3859999999999999</v>
       </c>
-      <c r="F22" s="4">
-        <f t="shared" ref="F22:Y22" si="2">F7*$C7</f>
+      <c r="F23" s="4">
+        <f t="shared" ref="F23:Y23" si="2">F7*$C7</f>
         <v>1.2044999999999999</v>
       </c>
-      <c r="G22" s="4">
-        <f t="shared" ref="G22" si="3">G7*$C7</f>
-        <v>0</v>
-      </c>
-      <c r="H22" s="4">
+      <c r="G23" s="4">
+        <f t="shared" ref="G23" si="3">G7*$C7</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M22" s="4">
+      <c r="M23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N22" s="4">
+      <c r="N23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O22" s="4">
+      <c r="O23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="P22" s="4">
+      <c r="P23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Q22" s="4">
+      <c r="Q23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="R22" s="4">
+      <c r="R23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="S22" s="4">
+      <c r="S23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="T22" s="4">
+      <c r="T23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="U22" s="4">
+      <c r="U23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="V22" s="4">
+      <c r="V23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="W22" s="4">
+      <c r="W23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="X22" s="4">
+      <c r="X23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="Y22" s="4">
+      <c r="Y23" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="AA22" s="4">
-        <f>SUM(E22:Y22)</f>
+      <c r="AA23" s="4">
+        <f>SUM(E23:Y23)</f>
         <v>2.5904999999999996</v>
       </c>
     </row>
-    <row r="23" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D23" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="4">
-        <f t="shared" ref="E23:Y23" si="4">E8*$C8</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="4">
+    <row r="24" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D24" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <f t="shared" ref="E24:Y24" si="4">E8*$C8</f>
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G23" s="4">
-        <f t="shared" ref="G23" si="5">G8*$C8</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
+      <c r="G24" s="4">
+        <f t="shared" ref="G24" si="5">G8*$C8</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="M23" s="4">
+      <c r="M24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="N23" s="4">
+      <c r="N24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="O23" s="4">
+      <c r="O24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="P23" s="4">
+      <c r="P24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="Q23" s="4">
+      <c r="Q24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="R23" s="4">
+      <c r="R24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="S23" s="4">
+      <c r="S24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="T23" s="4">
+      <c r="T24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="U23" s="4">
+      <c r="U24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="V23" s="4">
+      <c r="V24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="W23" s="4">
+      <c r="W24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="X23" s="4">
+      <c r="X24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="Y23" s="4">
+      <c r="Y24" s="4">
         <f t="shared" si="4"/>
         <v>3.3000000000000003</v>
       </c>
-      <c r="AA23" s="4">
-        <f>SUM(E23:Y23)</f>
+      <c r="AA24" s="4">
+        <f>SUM(E24:Y24)</f>
         <v>56.09999999999998</v>
       </c>
     </row>
-    <row r="24" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D24" s="21" t="s">
+    <row r="25" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D25" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E24" s="4">
-        <f t="shared" ref="E24:Y24" si="6">E9*$C9</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="4">
+      <c r="E25" s="4">
+        <f t="shared" ref="E25:Y25" si="6">E9*$C9</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="G24" s="4">
-        <f t="shared" ref="G24" si="7">G9*$C9</f>
-        <v>0</v>
-      </c>
-      <c r="H24" s="4">
+      <c r="G25" s="4">
+        <f t="shared" ref="G25" si="7">G9*$C9</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="4">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="M24" s="4">
+      <c r="M25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="N24" s="4">
+      <c r="N25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="O24" s="4">
+      <c r="O25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="P24" s="4">
+      <c r="P25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="Q24" s="4">
+      <c r="Q25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="R24" s="4">
+      <c r="R25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="S24" s="4">
+      <c r="S25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="T24" s="4">
+      <c r="T25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="U24" s="4">
+      <c r="U25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="V24" s="4">
+      <c r="V25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="W24" s="4">
+      <c r="W25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="X24" s="4">
+      <c r="X25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="Y24" s="4">
+      <c r="Y25" s="4">
         <f t="shared" si="6"/>
         <v>0.3</v>
       </c>
-      <c r="AA24" s="4">
-        <f t="shared" ref="AA24:AA28" si="8">SUM(E24:Y24)</f>
+      <c r="AA25" s="4">
+        <f t="shared" ref="AA25:AA29" si="8">SUM(E25:Y25)</f>
         <v>5.0999999999999988</v>
       </c>
     </row>
-    <row r="25" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D25" s="21" t="s">
+    <row r="26" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D26" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="4">
-        <f t="shared" ref="E25:Y25" si="9">E11*$C11</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="E26" s="4">
+        <f t="shared" ref="E26:Y26" si="9">E12*$C12</f>
+        <v>0</v>
+      </c>
+      <c r="F26" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G25" s="4">
-        <f t="shared" ref="G25" si="10">G11*$C11</f>
-        <v>0</v>
-      </c>
-      <c r="H25" s="4">
+      <c r="G26" s="4">
+        <f t="shared" ref="G26" si="10">G12*$C12</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I26" s="4">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="M25" s="4">
+      <c r="M26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="N25" s="4">
+      <c r="N26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="O25" s="4">
+      <c r="O26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="P25" s="4">
+      <c r="P26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Q25" s="4">
+      <c r="Q26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="R25" s="4">
+      <c r="R26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="S25" s="4">
+      <c r="S26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="T25" s="4">
+      <c r="T26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="U25" s="4">
+      <c r="U26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="V25" s="4">
+      <c r="V26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="W25" s="4">
+      <c r="W26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="X25" s="4">
+      <c r="X26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Y25" s="4">
+      <c r="Y26" s="4">
         <f t="shared" si="9"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="AA25" s="4">
+      <c r="AA26" s="4">
         <f t="shared" si="8"/>
         <v>1.7712000000000001</v>
       </c>
     </row>
-    <row r="26" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D26" s="21" t="s">
+    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D27" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="4">
-        <f t="shared" ref="E26:Y26" si="11">E12*$C12</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="E27" s="4">
+        <f t="shared" ref="E27:Y27" si="11">E13*$C13</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G26" s="4">
-        <f t="shared" ref="G26" si="12">G12*$C12</f>
-        <v>0</v>
-      </c>
-      <c r="H26" s="4">
+      <c r="G27" s="4">
+        <f t="shared" ref="G27" si="12">G13*$C13</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I27" s="4">
         <f t="shared" si="11"/>
         <v>0.43740000000000007</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="M26" s="4">
+      <c r="M27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="N26" s="4">
+      <c r="N27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="O26" s="4">
+      <c r="O27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="P26" s="4">
+      <c r="P27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Q26" s="4">
+      <c r="Q27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="R26" s="4">
+      <c r="R27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="S26" s="4">
+      <c r="S27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="T26" s="4">
+      <c r="T27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="U26" s="4">
+      <c r="U27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="V26" s="4">
+      <c r="V27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="W26" s="4">
+      <c r="W27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="X26" s="4">
+      <c r="X27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Y26" s="4">
+      <c r="Y27" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="AA26" s="4">
+      <c r="AA27" s="4">
         <f t="shared" si="8"/>
         <v>2.2086000000000001</v>
       </c>
     </row>
-    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D27" s="21" t="s">
+    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D28" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E27" s="4">
-        <f t="shared" ref="E27:Y27" si="13">E13*$C13</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="4">
+      <c r="E28" s="4">
+        <f t="shared" ref="E28:Y28" si="13">E14*$C14</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G27" s="4">
-        <f t="shared" ref="G27" si="14">G13*$C13</f>
+      <c r="G28" s="4">
+        <f t="shared" ref="G28" si="14">G14*$C14</f>
         <v>2.16</v>
       </c>
-      <c r="H27" s="4">
+      <c r="H28" s="4">
         <f t="shared" si="13"/>
         <v>4.2768000000000006</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I28" s="4">
         <f t="shared" si="13"/>
         <v>0.43740000000000007</v>
       </c>
-      <c r="J27" s="5">
+      <c r="J28" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K28" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L28" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="M27" s="5">
+      <c r="M28" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="N27" s="5">
+      <c r="N28" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="O27" s="4">
+      <c r="O28" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="P27" s="4">
+      <c r="P28" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Q27" s="5">
+      <c r="Q28" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="R27" s="5">
+      <c r="R28" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="S27" s="4">
+      <c r="S28" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="T27" s="4">
+      <c r="T28" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="U27" s="5">
+      <c r="U28" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="V27" s="5">
+      <c r="V28" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="W27" s="4">
+      <c r="W28" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="X27" s="4">
+      <c r="X28" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Y27" s="5">
+      <c r="Y28" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="AA27" s="4">
+      <c r="AA28" s="4">
         <f t="shared" si="8"/>
         <v>18.732600000000005</v>
       </c>
     </row>
-    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D28" s="21" t="s">
+    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D29" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="E28" s="4">
-        <f t="shared" ref="E28:Y28" si="15">E14*$C14</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
+      <c r="E29" s="4">
+        <f t="shared" ref="E29:Y29" si="15">E15*$C15</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G28" s="4">
-        <f t="shared" ref="G28" si="16">G14*$C14</f>
-        <v>0</v>
-      </c>
-      <c r="H28" s="4">
+      <c r="G29" s="4">
+        <f t="shared" ref="G29" si="16">G15*$C15</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I29" s="4">
         <f t="shared" si="15"/>
         <v>0.43740000000000007</v>
       </c>
-      <c r="J28" s="6">
+      <c r="J29" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K29" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="L28" s="6">
+      <c r="L29" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="M28" s="6">
+      <c r="M29" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N29" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O29" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="P28" s="6">
+      <c r="P29" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="Q29" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="R28" s="6">
+      <c r="R29" s="6">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="S28" s="4">
+      <c r="S29" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="T28" s="4">
+      <c r="T29" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="U28" s="4">
+      <c r="U29" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="V28" s="4">
+      <c r="V29" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="W28" s="4">
+      <c r="W29" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="X28" s="4">
+      <c r="X29" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Y28" s="4">
+      <c r="Y29" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="AA28" s="4">
+      <c r="AA29" s="4">
         <f t="shared" si="8"/>
         <v>12.295799999999998</v>
       </c>
     </row>
-    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D29" s="21"/>
-    </row>
     <row r="30" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="21"/>
+    </row>
+    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D31" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E30" s="4">
-        <f>SUM(E22:E28)</f>
+      <c r="E31" s="4">
+        <f>SUM(E23:E29)</f>
         <v>1.3859999999999999</v>
       </c>
-      <c r="F30" s="4">
-        <f>SUM(F22:F28)</f>
+      <c r="F31" s="4">
+        <f>SUM(F23:F29)</f>
         <v>1.2044999999999999</v>
       </c>
-      <c r="G30" s="4">
-        <f>SUM(G22:G28)</f>
+      <c r="G31" s="4">
+        <f>SUM(G23:G29)</f>
         <v>2.16</v>
       </c>
-      <c r="H30" s="4">
-        <f t="shared" ref="H30:Y30" si="17">SUM(H22:H28)</f>
+      <c r="H31" s="4">
+        <f t="shared" ref="H31:Y31" si="17">SUM(H23:H29)</f>
         <v>4.2768000000000006</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I31" s="4">
         <f t="shared" si="17"/>
         <v>4.9122000000000003</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J31" s="4">
         <f t="shared" si="17"/>
         <v>6.5646000000000004</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K31" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L31" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="M30" s="4">
+      <c r="M31" s="4">
         <f t="shared" si="17"/>
         <v>6.5646000000000004</v>
       </c>
-      <c r="N30" s="4">
+      <c r="N31" s="4">
         <f t="shared" si="17"/>
         <v>6.5646000000000004</v>
       </c>
-      <c r="O30" s="4">
+      <c r="O31" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="P30" s="4">
+      <c r="P31" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="Q30" s="4">
+      <c r="Q31" s="4">
         <f t="shared" si="17"/>
         <v>6.5646000000000004</v>
       </c>
-      <c r="R30" s="4">
+      <c r="R31" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="S30" s="4">
+      <c r="S31" s="4">
         <f t="shared" si="17"/>
         <v>4.0427999999999997</v>
       </c>
-      <c r="T30" s="4">
+      <c r="T31" s="4">
         <f t="shared" si="17"/>
         <v>4.0427999999999997</v>
       </c>
-      <c r="U30" s="4">
+      <c r="U31" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="V30" s="4">
+      <c r="V31" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="W30" s="4">
+      <c r="W31" s="4">
         <f t="shared" si="17"/>
         <v>4.0427999999999997</v>
       </c>
-      <c r="X30" s="4">
+      <c r="X31" s="4">
         <f t="shared" si="17"/>
         <v>4.0427999999999997</v>
       </c>
-      <c r="Y30" s="4">
+      <c r="Y31" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="AA30">
-        <f>SUM(E30:Y30)</f>
+      <c r="AA31">
+        <f>SUM(E31:Y31)</f>
         <v>98.798700000000011</v>
       </c>
     </row>
-    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="Z31" t="s">
+    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="Z32" t="s">
         <v>28</v>
       </c>
-      <c r="AA31" s="7">
+      <c r="AA32" s="7">
         <v>0.9</v>
       </c>
     </row>
-    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="AA32">
-        <f>AA30/AA31</f>
+    <row r="33" spans="8:27" x14ac:dyDescent="0.25">
+      <c r="AA33">
+        <f>AA31/AA32</f>
         <v>109.77633333333334</v>
       </c>
     </row>
-    <row r="33" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="Z33" t="s">
+    <row r="34" spans="8:27" x14ac:dyDescent="0.25">
+      <c r="Z34" t="s">
         <v>30</v>
       </c>
-      <c r="AA33">
-        <f>AA32/48</f>
+      <c r="AA34">
+        <f>AA33/48</f>
         <v>2.2870069444444447</v>
       </c>
     </row>
-    <row r="34" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="O34" s="4"/>
-    </row>
-    <row r="38" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="O38" t="s">
+    <row r="35" spans="8:27" x14ac:dyDescent="0.25">
+      <c r="O35" s="4"/>
+    </row>
+    <row r="39" spans="8:27" x14ac:dyDescent="0.25">
+      <c r="O39" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="I39" t="s">
+    <row r="40" spans="8:27" x14ac:dyDescent="0.25">
+      <c r="I40" t="s">
         <v>37</v>
       </c>
-      <c r="J39" t="s">
+      <c r="J40" t="s">
         <v>38</v>
       </c>
-      <c r="K39" t="s">
+      <c r="K40" t="s">
         <v>39</v>
       </c>
-      <c r="O39" t="s">
+      <c r="O40" t="s">
         <v>53</v>
-      </c>
-    </row>
-    <row r="40" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H40" t="s">
-        <v>36</v>
-      </c>
-      <c r="I40">
-        <v>25</v>
-      </c>
-      <c r="J40">
-        <v>0.18820000000000001</v>
-      </c>
-      <c r="K40" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="41" spans="8:27" x14ac:dyDescent="0.25">
       <c r="H41" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="I41">
         <v>25</v>
       </c>
       <c r="J41">
-        <v>0.72370000000000001</v>
+        <v>0.18820000000000001</v>
       </c>
       <c r="K41" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="I43" t="s">
-        <v>27</v>
-      </c>
-      <c r="J43">
-        <f>SUM(J40:J41)</f>
-        <v>0.91190000000000004</v>
+    <row r="42" spans="8:27" x14ac:dyDescent="0.25">
+      <c r="H42" t="s">
+        <v>41</v>
+      </c>
+      <c r="I42">
+        <v>25</v>
+      </c>
+      <c r="J42">
+        <v>0.72370000000000001</v>
+      </c>
+      <c r="K42" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="44" spans="8:27" x14ac:dyDescent="0.25">
       <c r="I44" t="s">
+        <v>27</v>
+      </c>
+      <c r="J44">
+        <f>SUM(J41:J42)</f>
+        <v>0.91190000000000004</v>
+      </c>
+    </row>
+    <row r="45" spans="8:27" x14ac:dyDescent="0.25">
+      <c r="I45" t="s">
         <v>42</v>
       </c>
-      <c r="J44">
+      <c r="J45">
         <v>1.65</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="E19:Y19"/>
+    <mergeCell ref="E20:Y20"/>
     <mergeCell ref="E4:Y4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
* another commit from last night
</commit_message>
<xml_diff>
--- a/hardware/power_budget.xlsx
+++ b/hardware/power_budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel2\projects\copper_suicide\hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel\projects\copper-suicide\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>VCC</t>
   </si>
@@ -116,9 +116,6 @@
     <t>MCU</t>
   </si>
   <si>
-    <t>I @ 48V</t>
-  </si>
-  <si>
     <t>SDRAM x16</t>
   </si>
   <si>
@@ -192,12 +189,18 @@
   </si>
   <si>
     <t>V12</t>
+  </si>
+  <si>
+    <t>primary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -406,7 +409,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -418,9 +421,6 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -441,6 +441,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -723,10 +727,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:AG45"/>
+  <dimension ref="B4:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Z18" sqref="Z18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,144 +744,144 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="27"/>
+      <c r="R4" s="27"/>
+      <c r="S4" s="27"/>
+      <c r="T4" s="27"/>
+      <c r="U4" s="27"/>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="27"/>
+      <c r="Y4" s="27"/>
       <c r="AA4" s="3"/>
-      <c r="AB4" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC4" s="24" t="s">
+      <c r="AB4" s="23" t="s">
         <v>47</v>
+      </c>
+      <c r="AC4" s="23" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="2:33" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H5" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" s="10" t="s">
+      <c r="F5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I5" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="O5" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="R5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="S5" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="T5" s="10" t="s">
+      <c r="T5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="U5" s="10" t="s">
+      <c r="U5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="V5" s="10" t="s">
+      <c r="V5" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="W5" s="10" t="s">
+      <c r="W5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="X5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="Y5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="AA5" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="AB5" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="AC5" s="24" t="s">
+      <c r="AA5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC5" s="23" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="D6" s="22"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="23"/>
-      <c r="W6" s="23"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+      <c r="G6" s="22"/>
+      <c r="H6" s="22"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="22"/>
+      <c r="K6" s="22"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22"/>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
     </row>
     <row r="7" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>3.3</v>
       </c>
-      <c r="D7" s="21" t="s">
-        <v>34</v>
+      <c r="D7" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="E7">
         <v>0.42</v>
@@ -942,19 +946,19 @@
       <c r="Y7">
         <v>0</v>
       </c>
-      <c r="AA7" s="19">
+      <c r="AA7" s="18">
         <f>SUM(E7:Y7)</f>
         <v>0.78499999999999992</v>
       </c>
-      <c r="AB7" s="18">
+      <c r="AB7" s="17">
         <f>AA7</f>
         <v>0.78499999999999992</v>
       </c>
-      <c r="AC7" s="17">
+      <c r="AC7" s="16">
         <v>1.5</v>
       </c>
-      <c r="AD7" s="11" t="s">
-        <v>43</v>
+      <c r="AD7" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="AE7">
         <f>AC7*3.3</f>
@@ -965,7 +969,7 @@
       <c r="C8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="20" t="s">
         <v>0</v>
       </c>
       <c r="E8">
@@ -1031,20 +1035,20 @@
       <c r="Y8">
         <v>3</v>
       </c>
-      <c r="AA8" s="19">
+      <c r="AA8" s="18">
         <f>SUM(E8:Y8)</f>
         <v>51</v>
       </c>
-      <c r="AB8" s="18">
+      <c r="AB8" s="17">
         <f>AA8</f>
         <v>51</v>
       </c>
-      <c r="AC8" s="17">
+      <c r="AC8" s="16">
         <f>3*17</f>
         <v>51</v>
       </c>
-      <c r="AD8" s="11" t="s">
-        <v>43</v>
+      <c r="AD8" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="AE8">
         <f>AC8*1.1</f>
@@ -1055,7 +1059,7 @@
       <c r="C9">
         <v>2.5</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>1</v>
       </c>
       <c r="E9">
@@ -1121,19 +1125,19 @@
       <c r="Y9">
         <v>0.12</v>
       </c>
-      <c r="AA9" s="19">
+      <c r="AA9" s="18">
         <f t="shared" ref="AA9:AA15" si="0">SUM(E9:Y9)</f>
         <v>2.0400000000000009</v>
       </c>
-      <c r="AB9" s="18">
+      <c r="AB9" s="17">
         <f>AA9</f>
         <v>2.0400000000000009</v>
       </c>
-      <c r="AC9" s="17">
+      <c r="AC9" s="16">
         <v>3</v>
       </c>
-      <c r="AD9" s="11" t="s">
-        <v>43</v>
+      <c r="AD9" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="AE9">
         <f>AC9*2.5</f>
@@ -1144,8 +1148,8 @@
       <c r="C10">
         <v>12</v>
       </c>
-      <c r="D10" s="21" t="s">
-        <v>55</v>
+      <c r="D10" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1210,17 +1214,17 @@
       <c r="Y10">
         <v>0</v>
       </c>
-      <c r="AA10" s="19">
+      <c r="AA10" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="18">
+      <c r="AB10" s="17">
         <f>AA10</f>
         <v>0</v>
       </c>
-      <c r="AC10" s="17"/>
-      <c r="AD10" s="26" t="s">
-        <v>43</v>
+      <c r="AC10" s="16"/>
+      <c r="AD10" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="AE10">
         <f>AC10*2.5</f>
@@ -1231,8 +1235,8 @@
       <c r="C11">
         <v>0.67500000000000004</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>51</v>
+      <c r="D11" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1297,19 +1301,19 @@
       <c r="Y11">
         <v>0</v>
       </c>
-      <c r="AA11" s="19">
+      <c r="AA11" s="18">
         <f t="shared" si="0"/>
         <v>1.6</v>
       </c>
-      <c r="AB11" s="18">
+      <c r="AB11" s="17">
         <f>AA11</f>
         <v>1.6</v>
       </c>
-      <c r="AC11" s="17">
+      <c r="AC11" s="16">
         <v>3</v>
       </c>
-      <c r="AD11" s="11" t="s">
-        <v>43</v>
+      <c r="AD11" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="AE11">
         <f>AC11*2.5</f>
@@ -1323,7 +1327,7 @@
       <c r="C12">
         <v>1.35</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="20" t="s">
         <v>2</v>
       </c>
       <c r="E12">
@@ -1341,55 +1345,55 @@
       <c r="I12">
         <v>0</v>
       </c>
-      <c r="J12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="K12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="L12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="M12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="N12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="O12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="P12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Q12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="R12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="S12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="T12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="U12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="V12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="W12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="X12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Y12" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="AA12" s="13">
+      <c r="J12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="K12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="L12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="N12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="O12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="P12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="R12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="S12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="V12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="W12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="X12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Y12" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AA12" s="12">
         <f t="shared" si="0"/>
         <v>1.3120000000000001</v>
       </c>
@@ -1401,7 +1405,7 @@
       <c r="C13">
         <v>1.35</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="20" t="s">
         <v>3</v>
       </c>
       <c r="E13">
@@ -1416,70 +1420,70 @@
       <c r="H13">
         <v>0</v>
       </c>
-      <c r="I13" s="12">
+      <c r="I13" s="11">
         <v>0.32400000000000001</v>
       </c>
-      <c r="J13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="K13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="L13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="M13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="N13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="O13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="P13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Q13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="R13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="S13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="T13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="U13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="V13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="W13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="X13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Y13" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="AA13" s="14">
+      <c r="J13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="K13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="L13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="M13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="N13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="O13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="P13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Q13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="R13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="S13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="V13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="W13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="X13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Y13" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AA13" s="13">
         <f t="shared" si="0"/>
         <v>1.6360000000000003</v>
       </c>
     </row>
     <row r="14" spans="2:33" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>44</v>
+      <c r="B14" s="11" t="s">
+        <v>43</v>
       </c>
       <c r="C14">
         <v>1.35</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>4</v>
       </c>
       <c r="E14">
@@ -1495,16 +1499,16 @@
         <f>0.198*16</f>
         <v>3.1680000000000001</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="11">
         <v>0.32400000000000001</v>
       </c>
       <c r="J14" s="2">
         <v>1.016</v>
       </c>
-      <c r="K14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="L14" s="20">
+      <c r="K14" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="L14" s="19">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="M14" s="2">
@@ -1513,10 +1517,10 @@
       <c r="N14" s="2">
         <v>1.016</v>
       </c>
-      <c r="O14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="P14" s="20">
+      <c r="O14" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="P14" s="19">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="Q14" s="2">
@@ -1525,10 +1529,10 @@
       <c r="R14" s="2">
         <v>1.016</v>
       </c>
-      <c r="S14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="T14" s="20">
+      <c r="S14" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T14" s="19">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="U14" s="2">
@@ -1537,16 +1541,16 @@
       <c r="V14" s="2">
         <v>1.016</v>
       </c>
-      <c r="W14" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="X14" s="20">
+      <c r="W14" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="X14" s="19">
         <v>8.2000000000000003E-2</v>
       </c>
       <c r="Y14" s="2">
         <v>1.016</v>
       </c>
-      <c r="AA14" s="14">
+      <c r="AA14" s="13">
         <f t="shared" si="0"/>
         <v>13.876000000000005</v>
       </c>
@@ -1554,13 +1558,13 @@
       <c r="AC14" s="4"/>
     </row>
     <row r="15" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="20" t="s">
-        <v>45</v>
+      <c r="B15" s="19" t="s">
+        <v>44</v>
       </c>
       <c r="C15">
         <v>1.35</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E15">
@@ -1575,7 +1579,7 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="11">
         <v>0.32400000000000001</v>
       </c>
       <c r="J15" s="8">
@@ -1599,46 +1603,46 @@
       <c r="P15" s="8">
         <v>1.016</v>
       </c>
-      <c r="Q15" s="27">
+      <c r="Q15" s="26">
         <v>1.016</v>
       </c>
-      <c r="R15" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="S15" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="T15" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="U15" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="V15" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="W15" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="X15" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="Y15" s="20">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="AA15" s="15">
+      <c r="R15" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="S15" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="T15" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="U15" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="V15" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="W15" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="X15" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="Y15" s="19">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AA15" s="14">
         <f t="shared" si="0"/>
         <v>9.1080000000000059</v>
       </c>
-      <c r="AB15" s="16">
+      <c r="AB15" s="15">
         <f>SUM(AA12:AA15)</f>
         <v>25.932000000000009</v>
       </c>
-      <c r="AC15" s="17">
+      <c r="AC15" s="16">
         <v>14</v>
       </c>
-      <c r="AD15" s="26" t="s">
-        <v>43</v>
+      <c r="AD15" s="25" t="s">
+        <v>42</v>
       </c>
       <c r="AE15">
         <f>AC15*2*1.35</f>
@@ -1655,156 +1659,162 @@
     </row>
     <row r="16" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="17" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="N17" s="25" t="s">
-        <v>50</v>
+      <c r="N17" s="24" t="s">
+        <v>49</v>
       </c>
       <c r="AF17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="4:32" x14ac:dyDescent="0.25">
       <c r="AF18" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="9"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
-      <c r="S20" s="9"/>
-      <c r="T20" s="9"/>
-      <c r="U20" s="9"/>
-      <c r="V20" s="9"/>
-      <c r="W20" s="9"/>
-      <c r="X20" s="9"/>
-      <c r="Y20" s="9"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="27"/>
+      <c r="T20" s="27"/>
+      <c r="U20" s="27"/>
+      <c r="V20" s="27"/>
+      <c r="W20" s="27"/>
+      <c r="X20" s="27"/>
+      <c r="Y20" s="27"/>
     </row>
     <row r="21" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="E21" s="10" t="str">
+      <c r="E21" s="9" t="str">
         <f>E5</f>
         <v>MCU</v>
       </c>
-      <c r="F21" s="10" t="str">
+      <c r="F21" s="9" t="str">
         <f>F5</f>
         <v>Clock Buffer</v>
       </c>
-      <c r="G21" s="10" t="str">
+      <c r="G21" s="9" t="str">
         <f>G5</f>
         <v>Misc</v>
       </c>
-      <c r="H21" s="10" t="str">
+      <c r="H21" s="9" t="str">
         <f t="shared" ref="H21:Y21" si="1">H5</f>
         <v>SDRAM x16</v>
       </c>
-      <c r="I21" s="10" t="str">
+      <c r="I21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-CFG</v>
       </c>
-      <c r="J21" s="10" t="str">
+      <c r="J21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-00</v>
       </c>
-      <c r="K21" s="10" t="str">
+      <c r="K21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-01</v>
       </c>
-      <c r="L21" s="10" t="str">
+      <c r="L21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-02</v>
       </c>
-      <c r="M21" s="10" t="str">
+      <c r="M21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-03</v>
       </c>
-      <c r="N21" s="10" t="str">
+      <c r="N21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-30</v>
       </c>
-      <c r="O21" s="10" t="str">
+      <c r="O21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-31</v>
       </c>
-      <c r="P21" s="10" t="str">
+      <c r="P21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-32</v>
       </c>
-      <c r="Q21" s="10" t="str">
+      <c r="Q21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-33</v>
       </c>
-      <c r="R21" s="10" t="str">
+      <c r="R21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-10</v>
       </c>
-      <c r="S21" s="10" t="str">
+      <c r="S21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-11</v>
       </c>
-      <c r="T21" s="10" t="str">
+      <c r="T21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-12</v>
       </c>
-      <c r="U21" s="10" t="str">
+      <c r="U21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-13</v>
       </c>
-      <c r="V21" s="10" t="str">
+      <c r="V21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-20</v>
       </c>
-      <c r="W21" s="10" t="str">
+      <c r="W21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-21</v>
       </c>
-      <c r="X21" s="10" t="str">
+      <c r="X21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-22</v>
       </c>
-      <c r="Y21" s="10" t="str">
+      <c r="Y21" s="9" t="str">
         <f t="shared" si="1"/>
         <v>FPGA-23</v>
       </c>
+      <c r="AA21" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB21" s="9" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="22" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D22" s="22"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
-      <c r="O22" s="23"/>
-      <c r="P22" s="23"/>
-      <c r="Q22" s="23"/>
-      <c r="R22" s="23"/>
-      <c r="S22" s="23"/>
-      <c r="T22" s="23"/>
-      <c r="U22" s="23"/>
-      <c r="V22" s="23"/>
-      <c r="W22" s="23"/>
-      <c r="X22" s="23"/>
-      <c r="Y22" s="23"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
+      <c r="T22" s="22"/>
+      <c r="U22" s="22"/>
+      <c r="V22" s="22"/>
+      <c r="W22" s="22"/>
+      <c r="X22" s="22"/>
+      <c r="Y22" s="22"/>
     </row>
     <row r="23" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D23" s="21" t="s">
-        <v>34</v>
+      <c r="D23" s="20" t="s">
+        <v>33</v>
       </c>
       <c r="E23" s="4">
         <f>E7*$C7</f>
@@ -1894,9 +1904,12 @@
         <f>SUM(E23:Y23)</f>
         <v>2.5904999999999996</v>
       </c>
+      <c r="AB23" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="24" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="20" t="s">
         <v>0</v>
       </c>
       <c r="E24" s="4">
@@ -1987,13 +2000,16 @@
         <f>SUM(E24:Y24)</f>
         <v>56.09999999999998</v>
       </c>
+      <c r="AB24" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="25" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="20" t="s">
         <v>1</v>
       </c>
       <c r="E25" s="4">
-        <f t="shared" ref="E25:Y25" si="6">E9*$C9</f>
+        <f t="shared" ref="E25:Y27" si="6">E9*$C9</f>
         <v>0</v>
       </c>
       <c r="F25" s="4">
@@ -2001,7 +2017,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="4">
-        <f t="shared" ref="G25" si="7">G9*$C9</f>
+        <f t="shared" ref="G25:G27" si="7">G9*$C9</f>
         <v>0</v>
       </c>
       <c r="H25" s="4">
@@ -2077,565 +2093,761 @@
         <v>0.3</v>
       </c>
       <c r="AA25" s="4">
-        <f t="shared" ref="AA25:AA29" si="8">SUM(E25:Y25)</f>
+        <f t="shared" ref="AA25:AA31" si="8">SUM(E25:Y25)</f>
         <v>5.0999999999999988</v>
       </c>
+      <c r="AB25" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="26" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D26" s="21" t="s">
-        <v>2</v>
+      <c r="D26" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="E26" s="4">
-        <f t="shared" ref="E26:Y26" si="9">E12*$C12</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="F26" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G26" s="4">
-        <f t="shared" ref="G26" si="10">G12*$C12</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="H26" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="I26" s="4">
-        <f t="shared" si="9"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="K26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="L26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="M26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="N26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="O26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="P26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="Q26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="R26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="S26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="T26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="U26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="V26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="W26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="X26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="Y26" s="4">
-        <f t="shared" si="9"/>
-        <v>0.11070000000000001</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="AA26" s="4">
         <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D27" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="4">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="4">
+        <f t="shared" si="6"/>
+        <v>1.08</v>
+      </c>
+      <c r="I27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Q27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="R27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="S27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="T27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="U27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="V27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="W27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="X27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="Y27" s="4">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AA27" s="4">
+        <f t="shared" si="8"/>
+        <v>1.08</v>
+      </c>
+    </row>
+    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D28" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4">
+        <f t="shared" ref="E28:Y28" si="9">E12*$C12</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="4">
+        <f t="shared" ref="G28" si="10">G12*$C12</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="4">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="K28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="L28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="M28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="N28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="O28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="P28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="Q28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="R28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="S28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="T28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="U28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="V28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="W28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="X28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="Y28" s="4">
+        <f t="shared" si="9"/>
+        <v>0.11070000000000001</v>
+      </c>
+      <c r="AA28" s="4">
+        <f t="shared" si="8"/>
         <v>1.7712000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D27" s="21" t="s">
+      <c r="AB28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D29" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E27" s="4">
-        <f t="shared" ref="E27:Y27" si="11">E13*$C13</f>
-        <v>0</v>
-      </c>
-      <c r="F27" s="4">
+      <c r="E29" s="4">
+        <f t="shared" ref="E29:Y29" si="11">E13*$C13</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="G27" s="4">
-        <f t="shared" ref="G27" si="12">G13*$C13</f>
-        <v>0</v>
-      </c>
-      <c r="H27" s="4">
+      <c r="G29" s="4">
+        <f t="shared" ref="G29" si="12">G13*$C13</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="4">
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I29" s="4">
         <f t="shared" si="11"/>
         <v>0.43740000000000007</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="M27" s="4">
+      <c r="M29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="N27" s="4">
+      <c r="N29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="O27" s="4">
+      <c r="O29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="P27" s="4">
+      <c r="P29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Q27" s="4">
+      <c r="Q29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="R27" s="4">
+      <c r="R29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="S27" s="4">
+      <c r="S29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="T27" s="4">
+      <c r="T29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="U27" s="4">
+      <c r="U29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="V27" s="4">
+      <c r="V29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="W27" s="4">
+      <c r="W29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="X27" s="4">
+      <c r="X29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Y27" s="4">
+      <c r="Y29" s="4">
         <f t="shared" si="11"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="AA27" s="4">
+      <c r="AA29" s="4">
         <f t="shared" si="8"/>
         <v>2.2086000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D28" s="21" t="s">
+      <c r="AB29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D30" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E28" s="4">
-        <f t="shared" ref="E28:Y28" si="13">E14*$C14</f>
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
+      <c r="E30" s="4">
+        <f t="shared" ref="E30:Y30" si="13">E14*$C14</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="4">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="G28" s="4">
-        <f t="shared" ref="G28" si="14">G14*$C14</f>
+      <c r="G30" s="4">
+        <f t="shared" ref="G30" si="14">G14*$C14</f>
         <v>2.16</v>
       </c>
-      <c r="H28" s="4">
+      <c r="H30" s="4">
         <f t="shared" si="13"/>
         <v>4.2768000000000006</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I30" s="4">
         <f t="shared" si="13"/>
         <v>0.43740000000000007</v>
       </c>
-      <c r="J28" s="5">
+      <c r="J30" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K30" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L30" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="M28" s="5">
+      <c r="M30" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="N28" s="5">
+      <c r="N30" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="O28" s="4">
+      <c r="O30" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="P28" s="4">
+      <c r="P30" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Q28" s="5">
+      <c r="Q30" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="R28" s="5">
+      <c r="R30" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="S28" s="4">
+      <c r="S30" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="T28" s="4">
+      <c r="T30" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="U28" s="5">
+      <c r="U30" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="V28" s="5">
+      <c r="V30" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="W28" s="4">
+      <c r="W30" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="X28" s="4">
+      <c r="X30" s="4">
         <f t="shared" si="13"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Y28" s="5">
+      <c r="Y30" s="5">
         <f t="shared" si="13"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="AA28" s="4">
+      <c r="AA30" s="4">
         <f t="shared" si="8"/>
         <v>18.732600000000005</v>
       </c>
-    </row>
-    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D29" s="21" t="s">
+      <c r="AB30" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D31" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E29" s="4">
-        <f t="shared" ref="E29:Y29" si="15">E15*$C15</f>
-        <v>0</v>
-      </c>
-      <c r="F29" s="4">
+      <c r="E31" s="4">
+        <f t="shared" ref="E31:Y31" si="15">E15*$C15</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="4">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="G29" s="4">
-        <f t="shared" ref="G29" si="16">G15*$C15</f>
-        <v>0</v>
-      </c>
-      <c r="H29" s="4">
+      <c r="G31" s="4">
+        <f t="shared" ref="G31" si="16">G15*$C15</f>
+        <v>0</v>
+      </c>
+      <c r="H31" s="4">
         <f t="shared" si="15"/>
         <v>0</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I31" s="4">
         <f t="shared" si="15"/>
         <v>0.43740000000000007</v>
       </c>
-      <c r="J29" s="6">
+      <c r="J31" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="K29" s="6">
+      <c r="K31" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="L29" s="6">
+      <c r="L31" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="M29" s="6">
+      <c r="M31" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N31" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="O29" s="6">
+      <c r="O31" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="P29" s="6">
+      <c r="P31" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="Q29" s="6">
+      <c r="Q31" s="6">
         <f t="shared" si="15"/>
         <v>1.3716000000000002</v>
       </c>
-      <c r="R29" s="6">
+      <c r="R31" s="6">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="S29" s="4">
+      <c r="S31" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="T29" s="4">
+      <c r="T31" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="U29" s="4">
+      <c r="U31" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="V29" s="4">
+      <c r="V31" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="W29" s="4">
+      <c r="W31" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="X29" s="4">
+      <c r="X31" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="Y29" s="4">
+      <c r="Y31" s="4">
         <f t="shared" si="15"/>
         <v>0.11070000000000001</v>
       </c>
-      <c r="AA29" s="4">
+      <c r="AA31" s="4">
         <f t="shared" si="8"/>
         <v>12.295799999999998</v>
       </c>
-    </row>
-    <row r="30" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D30" s="21"/>
-    </row>
-    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="D31" s="21" t="s">
+      <c r="AB31" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="D32" s="20"/>
+    </row>
+    <row r="33" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="D33" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="E31" s="4">
-        <f>SUM(E23:E29)</f>
+      <c r="E33" s="4">
+        <f>SUM(E23:E31)</f>
         <v>1.3859999999999999</v>
       </c>
-      <c r="F31" s="4">
-        <f>SUM(F23:F29)</f>
+      <c r="F33" s="4">
+        <f>SUM(F23:F31)</f>
         <v>1.2044999999999999</v>
       </c>
-      <c r="G31" s="4">
-        <f>SUM(G23:G29)</f>
+      <c r="G33" s="4">
+        <f>SUM(G23:G31)</f>
         <v>2.16</v>
       </c>
-      <c r="H31" s="4">
-        <f t="shared" ref="H31:Y31" si="17">SUM(H23:H29)</f>
-        <v>4.2768000000000006</v>
-      </c>
-      <c r="I31" s="4">
+      <c r="H33" s="4">
+        <f t="shared" ref="H33:Y33" si="17">SUM(H23:H31)</f>
+        <v>5.3568000000000007</v>
+      </c>
+      <c r="I33" s="4">
         <f t="shared" si="17"/>
         <v>4.9122000000000003</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J33" s="4">
         <f t="shared" si="17"/>
         <v>6.5646000000000004</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K33" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L33" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="M31" s="4">
+      <c r="M33" s="4">
         <f t="shared" si="17"/>
         <v>6.5646000000000004</v>
       </c>
-      <c r="N31" s="4">
+      <c r="N33" s="4">
         <f t="shared" si="17"/>
         <v>6.5646000000000004</v>
       </c>
-      <c r="O31" s="4">
+      <c r="O33" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="P31" s="4">
+      <c r="P33" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="Q31" s="4">
+      <c r="Q33" s="4">
         <f t="shared" si="17"/>
         <v>6.5646000000000004</v>
       </c>
-      <c r="R31" s="4">
+      <c r="R33" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="S31" s="4">
+      <c r="S33" s="4">
         <f t="shared" si="17"/>
         <v>4.0427999999999997</v>
       </c>
-      <c r="T31" s="4">
+      <c r="T33" s="4">
         <f t="shared" si="17"/>
         <v>4.0427999999999997</v>
       </c>
-      <c r="U31" s="4">
+      <c r="U33" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="V31" s="4">
+      <c r="V33" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="W31" s="4">
+      <c r="W33" s="4">
         <f t="shared" si="17"/>
         <v>4.0427999999999997</v>
       </c>
-      <c r="X31" s="4">
+      <c r="X33" s="4">
         <f t="shared" si="17"/>
         <v>4.0427999999999997</v>
       </c>
-      <c r="Y31" s="4">
+      <c r="Y33" s="4">
         <f t="shared" si="17"/>
         <v>5.3037000000000001</v>
       </c>
-      <c r="AA31">
-        <f>SUM(E31:Y31)</f>
-        <v>98.798700000000011</v>
-      </c>
-    </row>
-    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="Z32" t="s">
+      <c r="AC33" s="4">
+        <f>AA31+AA30+AA29+AA28+AA25+AA24+AA23</f>
+        <v>98.798699999999982</v>
+      </c>
+    </row>
+    <row r="34" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="AA34" s="7"/>
+      <c r="AB34" t="s">
         <v>28</v>
       </c>
-      <c r="AA32" s="7">
+      <c r="AC34" s="7">
         <v>0.9</v>
       </c>
     </row>
-    <row r="33" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="AA33">
-        <f>AA31/AA32</f>
-        <v>109.77633333333334</v>
-      </c>
-    </row>
-    <row r="34" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="Z34" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA34">
-        <f>AA33/48</f>
-        <v>2.2870069444444447</v>
-      </c>
-    </row>
-    <row r="35" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="O35" s="4"/>
-    </row>
-    <row r="39" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="O39" t="s">
+    <row r="35" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="AB35" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC35" s="28">
+        <f>AC33/AC34</f>
+        <v>109.77633333333331</v>
+      </c>
+    </row>
+    <row r="37" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="O37" s="4"/>
+    </row>
+    <row r="41" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="O41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="I42" t="s">
+        <v>36</v>
+      </c>
+      <c r="J42" t="s">
+        <v>37</v>
+      </c>
+      <c r="K42" t="s">
+        <v>38</v>
+      </c>
+      <c r="O42" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="I40" t="s">
-        <v>37</v>
-      </c>
-      <c r="J40" t="s">
-        <v>38</v>
-      </c>
-      <c r="K40" t="s">
+    <row r="43" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="H43" t="s">
+        <v>35</v>
+      </c>
+      <c r="I43">
+        <v>25</v>
+      </c>
+      <c r="J43">
+        <v>0.18820000000000001</v>
+      </c>
+      <c r="K43" t="s">
         <v>39</v>
       </c>
-      <c r="O40" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="41" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H41" t="s">
-        <v>36</v>
-      </c>
-      <c r="I41">
+    </row>
+    <row r="44" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="H44" t="s">
+        <v>40</v>
+      </c>
+      <c r="I44">
         <v>25</v>
       </c>
-      <c r="J41">
-        <v>0.18820000000000001</v>
-      </c>
-      <c r="K41" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="H42" t="s">
+      <c r="J44">
+        <v>0.72370000000000001</v>
+      </c>
+      <c r="K44" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="46" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="I46" t="s">
+        <v>27</v>
+      </c>
+      <c r="J46">
+        <f>SUM(J43:J44)</f>
+        <v>0.91190000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="4:29" x14ac:dyDescent="0.25">
+      <c r="I47" t="s">
         <v>41</v>
       </c>
-      <c r="I42">
-        <v>25</v>
-      </c>
-      <c r="J42">
-        <v>0.72370000000000001</v>
-      </c>
-      <c r="K42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="44" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="I44" t="s">
-        <v>27</v>
-      </c>
-      <c r="J44">
-        <f>SUM(J41:J42)</f>
-        <v>0.91190000000000004</v>
-      </c>
-    </row>
-    <row r="45" spans="8:27" x14ac:dyDescent="0.25">
-      <c r="I45" t="s">
-        <v>42</v>
-      </c>
-      <c r="J45">
+      <c r="J47">
         <v>1.65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* nightly commit * BOM cleanup (still not done, and have not yet sync'd with PCB) * fixed 12V power supply
</commit_message>
<xml_diff>
--- a/hardware/power_budget.xlsx
+++ b/hardware/power_budget.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel\projects\copper-suicide\hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joel2\projects\copper_suicide\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>VCC</t>
   </si>
@@ -119,9 +119,6 @@
     <t>SDRAM x16</t>
   </si>
   <si>
-    <t>2.343 (3.3V SSTL)</t>
-  </si>
-  <si>
     <t>Clock Buffer</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
   </si>
   <si>
     <t>VTT Regulator (1.35V input)</t>
-  </si>
-  <si>
-    <t>0.779A (1.35V SSTL 50% TX/RX)</t>
   </si>
   <si>
     <t>V12</t>
@@ -199,9 +193,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -212,13 +206,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,7 +226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -261,11 +248,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
@@ -404,12 +386,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -421,9 +402,9 @@
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -431,23 +412,21 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -727,10 +706,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:AG47"/>
+  <dimension ref="B4:AD47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Z18" sqref="Z18"/>
+      <selection activeCell="S41" sqref="S41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -743,7 +722,7 @@
     <col min="9" max="9" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:30" x14ac:dyDescent="0.25">
       <c r="E4" s="27" t="s">
         <v>25</v>
       </c>
@@ -769,24 +748,24 @@
       <c r="Y4" s="27"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AC4" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="2:33" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>30</v>
@@ -843,16 +822,16 @@
         <v>18</v>
       </c>
       <c r="AA5" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB5" s="23" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AC5" s="23" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:30" x14ac:dyDescent="0.25">
       <c r="D6" s="21"/>
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
@@ -876,12 +855,12 @@
       <c r="X6" s="22"/>
       <c r="Y6" s="22"/>
     </row>
-    <row r="7" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>3.3</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E7">
         <v>0.42</v>
@@ -958,14 +937,10 @@
         <v>1.5</v>
       </c>
       <c r="AD7" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE7">
-        <f>AC7*3.3</f>
-        <v>4.9499999999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="2:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>1.1000000000000001</v>
       </c>
@@ -1048,14 +1023,10 @@
         <v>51</v>
       </c>
       <c r="AD8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE8">
-        <f>AC8*1.1</f>
-        <v>56.1</v>
-      </c>
-    </row>
-    <row r="9" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="2:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>2.5</v>
       </c>
@@ -1137,19 +1108,15 @@
         <v>3</v>
       </c>
       <c r="AD9" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE9">
-        <f>AC9*2.5</f>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="10" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="2:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>12</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1219,24 +1186,21 @@
         <v>0</v>
       </c>
       <c r="AB10" s="17">
-        <f>AA10</f>
-        <v>0</v>
-      </c>
-      <c r="AC10" s="16"/>
-      <c r="AD10" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE10">
-        <f>AC10*2.5</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>8.9499999999999993</v>
+      </c>
+      <c r="AC10" s="16">
+        <v>9</v>
+      </c>
+      <c r="AD10" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="2:30" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>0.67500000000000004</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1313,14 +1277,10 @@
         <v>3</v>
       </c>
       <c r="AD11" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE11">
-        <f>AC11*2.5</f>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="12" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="2:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1398,7 +1358,7 @@
         <v>1.3120000000000001</v>
       </c>
     </row>
-    <row r="13" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>23</v>
       </c>
@@ -1476,9 +1436,9 @@
         <v>1.6360000000000003</v>
       </c>
     </row>
-    <row r="14" spans="2:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B14" s="11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14">
         <v>1.35</v>
@@ -1557,9 +1517,9 @@
       <c r="AB14" s="4"/>
       <c r="AC14" s="4"/>
     </row>
-    <row r="15" spans="2:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15">
         <v>1.35</v>
@@ -1603,7 +1563,7 @@
       <c r="P15" s="8">
         <v>1.016</v>
       </c>
-      <c r="Q15" s="26">
+      <c r="Q15" s="25">
         <v>1.016</v>
       </c>
       <c r="R15" s="19">
@@ -1639,39 +1599,19 @@
         <v>25.932000000000009</v>
       </c>
       <c r="AC15" s="16">
-        <v>14</v>
-      </c>
-      <c r="AD15" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="AE15">
-        <f>AC15*2*1.35</f>
-        <v>37.800000000000004</v>
-      </c>
-      <c r="AF15">
-        <f>SUM(AE7:AE15)</f>
-        <v>113.85</v>
-      </c>
-      <c r="AG15">
-        <f>AF15/0.9</f>
-        <v>126.49999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="2:33" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="4:32" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="AD15" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="4:28" x14ac:dyDescent="0.25">
       <c r="N17" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="4:32" x14ac:dyDescent="0.25">
-      <c r="AF18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="4:32" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E20" s="27" t="s">
         <v>26</v>
       </c>
@@ -1696,7 +1636,7 @@
       <c r="X20" s="27"/>
       <c r="Y20" s="27"/>
     </row>
-    <row r="21" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:28" x14ac:dyDescent="0.25">
       <c r="E21" s="9" t="str">
         <f>E5</f>
         <v>MCU</v>
@@ -1782,13 +1722,13 @@
         <v>FPGA-23</v>
       </c>
       <c r="AA21" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="AB21" s="9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="22" spans="4:32" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D22" s="21"/>
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
@@ -1812,9 +1752,9 @@
       <c r="X22" s="22"/>
       <c r="Y22" s="22"/>
     </row>
-    <row r="23" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D23" s="20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="4">
         <f>E7*$C7</f>
@@ -1905,10 +1845,10 @@
         <v>2.5904999999999996</v>
       </c>
       <c r="AB23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="24" spans="4:32" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D24" s="20" t="s">
         <v>0</v>
       </c>
@@ -2001,10 +1941,10 @@
         <v>56.09999999999998</v>
       </c>
       <c r="AB24" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="25" spans="4:32" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D25" s="20" t="s">
         <v>1</v>
       </c>
@@ -2097,12 +2037,12 @@
         <v>5.0999999999999988</v>
       </c>
       <c r="AB25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="4:32" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D26" s="20" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E26" s="4">
         <f t="shared" si="6"/>
@@ -2193,9 +2133,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D27" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="6"/>
@@ -2286,7 +2226,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="28" spans="4:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D28" s="20" t="s">
         <v>2</v>
       </c>
@@ -2379,10 +2319,10 @@
         <v>1.7712000000000001</v>
       </c>
       <c r="AB28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="4:32" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D29" s="20" t="s">
         <v>3</v>
       </c>
@@ -2475,10 +2415,10 @@
         <v>2.2086000000000001</v>
       </c>
       <c r="AB29" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="30" spans="4:32" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D30" s="20" t="s">
         <v>4</v>
       </c>
@@ -2571,10 +2511,10 @@
         <v>18.732600000000005</v>
       </c>
       <c r="AB30" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="31" spans="4:32" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D31" s="20" t="s">
         <v>5</v>
       </c>
@@ -2667,10 +2607,10 @@
         <v>12.295799999999998</v>
       </c>
       <c r="AB31" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="4:32" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" spans="4:28" x14ac:dyDescent="0.25">
       <c r="D32" s="20"/>
     </row>
     <row r="33" spans="4:29" x14ac:dyDescent="0.25">
@@ -2772,16 +2712,16 @@
         <v>28</v>
       </c>
       <c r="AC34" s="7">
-        <v>0.9</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="35" spans="4:29" x14ac:dyDescent="0.25">
       <c r="AB35" t="s">
         <v>27</v>
       </c>
-      <c r="AC35" s="28">
+      <c r="AC35" s="26">
         <f>AC33/AC34</f>
-        <v>109.77633333333331</v>
+        <v>107.3898913043478</v>
       </c>
     </row>
     <row r="37" spans="4:29" x14ac:dyDescent="0.25">
@@ -2789,26 +2729,26 @@
     </row>
     <row r="41" spans="4:29" x14ac:dyDescent="0.25">
       <c r="O41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="4:29" x14ac:dyDescent="0.25">
       <c r="I42" t="s">
+        <v>35</v>
+      </c>
+      <c r="J42" t="s">
         <v>36</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>37</v>
       </c>
-      <c r="K42" t="s">
-        <v>38</v>
-      </c>
       <c r="O42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="43" spans="4:29" x14ac:dyDescent="0.25">
       <c r="H43" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I43">
         <v>25</v>
@@ -2817,12 +2757,12 @@
         <v>0.18820000000000001</v>
       </c>
       <c r="K43" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="4:29" x14ac:dyDescent="0.25">
       <c r="H44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I44">
         <v>25</v>
@@ -2831,7 +2771,7 @@
         <v>0.72370000000000001</v>
       </c>
       <c r="K44" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="4:29" x14ac:dyDescent="0.25">
@@ -2845,7 +2785,7 @@
     </row>
     <row r="47" spans="4:29" x14ac:dyDescent="0.25">
       <c r="I47" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J47">
         <v>1.65</v>

</xml_diff>